<commit_message>
ran evans 4 jobs, wont delete files
</commit_message>
<xml_diff>
--- a/autoast/test_2_shp_files_w_filenumber.xlsx
+++ b/autoast/test_2_shp_files_w_filenumber.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\Scripts\ast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\GitHubAutoAST\gss_authorizations\autoast\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>region</t>
   </si>
@@ -60,28 +60,34 @@
     <t>ast_condition</t>
   </si>
   <si>
-    <t>Northeast</t>
-  </si>
-  <si>
-    <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\FwToolOutputJuly23\876367\876367_300m_buffer.shp</t>
-  </si>
-  <si>
     <t>False</t>
   </si>
   <si>
     <t>True</t>
   </si>
   <si>
-    <t>\\spatialfiles.bcgov\work\srm\nel\Local\Geomatics\Workarea\csostad\WildLifePermittingTest\FwToolOutputJuly23\876372_v2\ChiefsCabinCreek_50m_buffer.shp</t>
-  </si>
-  <si>
     <t>file_number</t>
   </si>
   <si>
-    <t>T:\job1</t>
-  </si>
-  <si>
-    <t>T:\job2</t>
+    <t>Cariboo</t>
+  </si>
+  <si>
+    <t>\\spatialfiles.bcgov\Work\srm\wml\Workarea\Authorizations\Land\Cariboo\Cariboo_Batch_GR_20204_724\240263</t>
+  </si>
+  <si>
+    <t>\\spatialfiles.bcgov\Work\srm\wml\Workarea\Authorizations\Land\Cariboo\Cariboo_Batch_GR_20204_724\5407781</t>
+  </si>
+  <si>
+    <t>T:\job2\\spatialfiles.bcgov\Work\srm\wml\Workarea\Authorizations\Land\Cariboo\Cariboo_Batch_GR_20204_724\247611</t>
+  </si>
+  <si>
+    <t>\\spatialfiles.bcgov\Work\srm\wml\Workarea\Authorizations\Land\Cariboo\Cariboo_Batch_GR_20204_724\25407734</t>
+  </si>
+  <si>
+    <t>0247611</t>
+  </si>
+  <si>
+    <t>0240263</t>
   </si>
 </sst>
 </file>
@@ -435,17 +441,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="180.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="167.140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="117.5703125" customWidth="1"/>
     <col min="7" max="7" width="39" style="1" customWidth="1"/>
     <col min="8" max="8" width="25.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="32" style="1" customWidth="1"/>
@@ -462,7 +469,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -496,79 +503,163 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>949613</v>
+      </c>
+      <c r="E2">
+        <v>984515</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2">
-        <v>876372</v>
+        <v>13</v>
       </c>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>949614</v>
+      </c>
+      <c r="E3">
+        <v>984516</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="M3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5407734</v>
+      </c>
+      <c r="D4">
+        <v>949615</v>
+      </c>
+      <c r="E4">
+        <v>984517</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3">
-        <v>876367</v>
+      <c r="C5" s="1">
+        <v>5407781</v>
+      </c>
+      <c r="D5">
+        <v>949616</v>
+      </c>
+      <c r="E5">
+        <v>984518</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>